<commit_message>
Graphiques mis à jour
</commit_message>
<xml_diff>
--- a/papier/Analyses_graphiques/Data/Adblock2Ultimate_ghostery.xlsx
+++ b/papier/Analyses_graphiques/Data/Adblock2Ultimate_ghostery.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antoine\Desktop\Analyses_mémoire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Analyses_graphiques\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -204,20 +204,9 @@
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent1"/>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -230,20 +219,9 @@
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent2"/>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -256,20 +234,9 @@
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent3">
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent3"/>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -282,20 +249,9 @@
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent4">
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent4"/>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -308,20 +264,9 @@
             <c:idx val="4"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent5">
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent5"/>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -334,20 +279,9 @@
             <c:idx val="5"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent6">
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent6"/>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -360,23 +294,11 @@
             <c:idx val="6"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="60000"/>
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="60000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -389,23 +311,11 @@
             <c:idx val="7"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="60000"/>
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="60000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -418,23 +328,11 @@
             <c:idx val="8"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent3">
-                      <a:lumMod val="60000"/>
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent3">
-                      <a:lumMod val="60000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -447,23 +345,11 @@
             <c:idx val="9"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent4">
-                      <a:lumMod val="60000"/>
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent4">
-                      <a:lumMod val="60000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -476,23 +362,11 @@
             <c:idx val="10"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent5">
-                      <a:lumMod val="60000"/>
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent5">
-                      <a:lumMod val="60000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -505,23 +379,11 @@
             <c:idx val="11"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent6">
-                      <a:lumMod val="60000"/>
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent6">
-                      <a:lumMod val="60000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -534,25 +396,12 @@
             <c:idx val="12"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="80000"/>
-                      <a:lumOff val="20000"/>
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="80000"/>
-                      <a:lumOff val="20000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -565,25 +414,12 @@
             <c:idx val="13"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="80000"/>
-                      <a:lumOff val="20000"/>
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="80000"/>
-                      <a:lumOff val="20000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -596,25 +432,12 @@
             <c:idx val="14"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent3">
-                      <a:lumMod val="80000"/>
-                      <a:lumOff val="20000"/>
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent3">
-                      <a:lumMod val="80000"/>
-                      <a:lumOff val="20000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -627,25 +450,12 @@
             <c:idx val="15"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent4">
-                      <a:lumMod val="80000"/>
-                      <a:lumOff val="20000"/>
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent4">
-                      <a:lumMod val="80000"/>
-                      <a:lumOff val="20000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -658,25 +468,12 @@
             <c:idx val="16"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent5">
-                      <a:lumMod val="80000"/>
-                      <a:lumOff val="20000"/>
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent5">
-                      <a:lumMod val="80000"/>
-                      <a:lumOff val="20000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -689,25 +486,12 @@
             <c:idx val="17"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent6">
-                      <a:lumMod val="80000"/>
-                      <a:lumOff val="20000"/>
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent6">
-                      <a:lumMod val="80000"/>
-                      <a:lumOff val="20000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
@@ -731,11 +515,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="dk1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -758,7 +542,7 @@
               <c:spPr>
                 <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                   <a:solidFill>
-                    <a:schemeClr val="dk1">
+                    <a:schemeClr val="tx1">
                       <a:lumMod val="35000"/>
                       <a:lumOff val="65000"/>
                     </a:schemeClr>
@@ -912,7 +696,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
+                <a:schemeClr val="tx1">
                   <a:lumMod val="35000"/>
                   <a:lumOff val="65000"/>
                 </a:schemeClr>
@@ -932,15 +716,11 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -951,9 +731,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
@@ -972,20 +752,12 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:pattFill prst="dkDnDiag">
-      <a:fgClr>
-        <a:schemeClr val="lt1"/>
-      </a:fgClr>
-      <a:bgClr>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="10000"/>
-          <a:lumOff val="90000"/>
-        </a:schemeClr>
-      </a:bgClr>
-    </a:pattFill>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="dk1">
+        <a:schemeClr val="tx1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1048,8 +820,78 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="337">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="333">
   <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1059,84 +901,15 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="dkDnDiag">
-        <a:fgClr>
-          <a:schemeClr val="lt1"/>
-        </a:fgClr>
-        <a:bgClr>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="10000"/>
-            <a:lumOff val="90000"/>
-          </a:schemeClr>
-        </a:bgClr>
-      </a:pattFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:alpha val="75000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1156,20 +929,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="phClr">
-              <a:lumMod val="60000"/>
-              <a:lumOff val="40000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="phClr"/>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="19050">
         <a:solidFill>
           <a:schemeClr val="lt1"/>
@@ -1187,21 +949,10 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="phClr">
-              <a:lumMod val="60000"/>
-              <a:lumOff val="40000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="phClr"/>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-      <a:ln w="50800">
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
         <a:solidFill>
           <a:schemeClr val="lt1"/>
         </a:solidFill>
@@ -1215,10 +966,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1227,25 +978,22 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
+    <cs:lnRef idx="0"/>
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="15875">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
@@ -1257,7 +1005,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1273,15 +1021,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
+      <a:noFill/>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1289,14 +1038,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="800" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1307,7 +1056,116 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
@@ -1315,18 +1173,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -1334,83 +1192,58 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -1418,103 +1251,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:alpha val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="major">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="0" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1440" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1523,13 +1271,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1538,7 +1287,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -1550,7 +1299,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1558,9 +1307,9 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1572,7 +1321,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -1584,8 +1333,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1594,7 +1349,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1605,7 +1360,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9296797" cy="6072188"/>
+    <xdr:ext cx="9294725" cy="6070879"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1"/>

</xml_diff>